<commit_message>
Deleted copy of dncp-scrapper and added example of openpyxl
</commit_message>
<xml_diff>
--- a/Python/Drive+Scrap/123.xlsx
+++ b/Python/Drive+Scrap/123.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8514" uniqueCount="1534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8514" uniqueCount="1535">
   <si>
     <t>IdentificaciÃ³n / Nombre del solicitante</t>
   </si>
@@ -4621,6 +4621,9 @@
   </si>
   <si>
     <t>Nro</t>
+  </si>
+  <si>
+    <t>abr prro</t>
   </si>
 </sst>
 </file>
@@ -5430,7 +5433,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF329"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -5540,7 +5545,7 @@
         <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>1534</v>
       </c>
       <c r="D2" t="s">
         <v>33</v>

</xml_diff>